<commit_message>
Updated with RevC hardware
</commit_message>
<xml_diff>
--- a/Mussel_heartrate_module/Mussel_heartrate_module_parts.xlsx
+++ b/Mussel_heartrate_module/Mussel_heartrate_module_parts.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5674ADED-4EA5-40D6-A990-3AE964124843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="11350" yWindow="710" windowWidth="22410" windowHeight="18490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RevA" sheetId="1" r:id="rId1"/>
+    <sheet name="RevC" sheetId="3" r:id="rId1"/>
+    <sheet name="RevA-B" sheetId="1" r:id="rId2"/>
+    <sheet name="Reference_design" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
   <si>
     <t>Description</t>
   </si>
@@ -171,18 +174,12 @@
     <t>C3,C4</t>
   </si>
   <si>
-    <t>RevA, RevB parts</t>
-  </si>
-  <si>
     <t>1.8V voltage regulator Microchip MIC5365</t>
   </si>
   <si>
     <t>Level shifter, Texas Inst. 8-VSSOP</t>
   </si>
   <si>
-    <t xml:space="preserve"> MIC5365-1.8YC5-TR</t>
-  </si>
-  <si>
     <t>GRM155R70G105KA12D</t>
   </si>
   <si>
@@ -190,12 +187,108 @@
   </si>
   <si>
     <t>Capacitor, 1µF 10% 10V X7R 0402 Murata</t>
+  </si>
+  <si>
+    <t>576-3181-1-ND</t>
+  </si>
+  <si>
+    <t>2368-47-23348-CL-ND</t>
+  </si>
+  <si>
+    <t>Clear heat shrink - adhesive lined 3/8 diameter</t>
+  </si>
+  <si>
+    <t>47-23348-CL</t>
+  </si>
+  <si>
+    <t>HeartRate Sensor RevA, RevB parts</t>
+  </si>
+  <si>
+    <t>MAX30101 sensor 14-OESIP</t>
+  </si>
+  <si>
+    <t>MAX30101EFD+</t>
+  </si>
+  <si>
+    <t>MAX30101EFD+-ND</t>
+  </si>
+  <si>
+    <t>HeartRate Sensor RevC parts</t>
+  </si>
+  <si>
+    <t>VCNL4040M30E Proximity sensor</t>
+  </si>
+  <si>
+    <t>VCNL4040</t>
+  </si>
+  <si>
+    <t>VCNL4040M3OECT-ND</t>
+  </si>
+  <si>
+    <t>TMP117 temperature sensor</t>
+  </si>
+  <si>
+    <t>VCNL4040M3OE</t>
+  </si>
+  <si>
+    <t>TMP117MAIDRVR</t>
+  </si>
+  <si>
+    <t>TMP117</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
+  </si>
+  <si>
+    <t>R3, R4</t>
+  </si>
+  <si>
+    <t>RC0402JR-072K2L</t>
+  </si>
+  <si>
+    <t>311-2.2KJRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402JR-0722RL</t>
+  </si>
+  <si>
+    <t>311-22JRCT-ND</t>
+  </si>
+  <si>
+    <t>22 ohm resistor 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>2.2k ohm resistor 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>C1005X7R1C104K050BC</t>
+  </si>
+  <si>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>Capacitor, 2.2µF 16V 10% X7R 0402</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C1005X7S1A225K050BC</t>
+  </si>
+  <si>
+    <t>445-9097-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = </t>
+  </si>
+  <si>
+    <t>296-52215-2-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -244,11 +337,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -529,11 +629,222 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067BA664-449E-467C-A1FC-C1A06CA73029}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="5"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="G3" s="1">
+        <f>F3*E3</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3.81</v>
+      </c>
+      <c r="G4" s="1">
+        <f>F4*E4</f>
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ref="G5:G8" si="0">F5*E5</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="4">
+        <f>SUM(G3:G8)</f>
+        <v>7.12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -545,10 +856,266 @@
     <col min="6" max="7" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="G4" s="1">
+        <f>F4*E4</f>
+        <v>8.9700000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.01</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ref="G5:G11" si="0">F5*E5</f>
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="3">
+        <f>SUM(G4:G11)</f>
+        <v>11.91</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="89" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -588,7 +1155,7 @@
         <v>4.51</v>
       </c>
       <c r="G3" s="1">
-        <f>F3*E3</f>
+        <f t="shared" ref="G3:G12" si="0">F3*E3</f>
         <v>4.51</v>
       </c>
     </row>
@@ -609,7 +1176,7 @@
         <v>2.27</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" ref="G4:G12" si="0">F4*E4</f>
+        <f t="shared" si="0"/>
         <v>2.27</v>
       </c>
     </row>
@@ -781,6 +1348,10 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F14" s="3" t="s">
         <v>26</v>
@@ -790,228 +1361,7 @@
         <v>11.729999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1">
-        <v>4.51</v>
-      </c>
-      <c r="G18" s="1">
-        <f>F18*E18</f>
-        <v>4.51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1.01</v>
-      </c>
-      <c r="G19" s="1">
-        <f t="shared" ref="G19:G25" si="1">F19*E19</f>
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="G20" s="1">
-        <f t="shared" si="1"/>
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="G21" s="1">
-        <f t="shared" si="1"/>
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0.27</v>
-      </c>
-      <c r="G22" s="1">
-        <f t="shared" si="1"/>
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="G23" s="1">
-        <f t="shared" si="1"/>
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-      <c r="F24" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="G24" s="1">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25">
-        <v>5</v>
-      </c>
-      <c r="F25" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="3">
-        <f>SUM(G18:G25)</f>
-        <v>7.45</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating sensor parts list - RevC
Added parts list for the VCNL4040-based RevC heart rate sensor board.
</commit_message>
<xml_diff>
--- a/Mussel_heartrate_module/Mussel_heartrate_module_parts.xlsx
+++ b/Mussel_heartrate_module/Mussel_heartrate_module_parts.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5674ADED-4EA5-40D6-A990-3AE964124843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3376C33-3EB8-4321-A317-E18723997348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11350" yWindow="710" windowWidth="22410" windowHeight="18490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="3660" windowWidth="18310" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RevC" sheetId="3" r:id="rId1"/>
@@ -630,10 +630,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067BA664-449E-467C-A1FC-C1A06CA73029}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G8" sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -831,8 +834,9 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updating with new parts
</commit_message>
<xml_diff>
--- a/Mussel_heartrate_module/Mussel_heartrate_module_parts.xlsx
+++ b/Mussel_heartrate_module/Mussel_heartrate_module_parts.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3376C33-3EB8-4321-A317-E18723997348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="3660" windowWidth="18310" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="3660" windowWidth="18310" windowHeight="16160"/>
   </bookViews>
   <sheets>
     <sheet name="RevC" sheetId="3" r:id="rId1"/>
@@ -288,7 +287,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -629,7 +628,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067BA664-449E-467C-A1FC-C1A06CA73029}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -841,7 +840,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1099,7 +1098,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Creating KiCad version of the hardware
</commit_message>
<xml_diff>
--- a/Mussel_heartrate_module/Mussel_heartrate_module_parts.xlsx
+++ b/Mussel_heartrate_module/Mussel_heartrate_module_parts.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73E264C-26E8-451B-8DC3-F0B870BD75EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="3660" windowWidth="18310" windowHeight="16160"/>
+    <workbookView xWindow="4690" yWindow="1090" windowWidth="32550" windowHeight="18540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RevC" sheetId="3" r:id="rId1"/>
     <sheet name="RevA-B" sheetId="1" r:id="rId2"/>
     <sheet name="Reference_design" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="95">
   <si>
     <t>Description</t>
   </si>
@@ -282,12 +293,36 @@
   </si>
   <si>
     <t>296-52215-2-ND</t>
+  </si>
+  <si>
+    <t>Alternate PN</t>
+  </si>
+  <si>
+    <t>Alternate Digikey PN</t>
+  </si>
+  <si>
+    <t>MAX30100EFD+TCT-ND</t>
+  </si>
+  <si>
+    <t>296-46571-1-ND</t>
+  </si>
+  <si>
+    <t>TCA9801DGKT</t>
+  </si>
+  <si>
+    <t>NCP508SQ18T1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>NCP508SQ18T1G</t>
+  </si>
+  <si>
+    <t>MAX30100EFD+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -628,13 +663,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
@@ -840,14 +875,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G13"/>
+  <dimension ref="A2:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -857,14 +892,16 @@
     <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="8.7265625" style="1"/>
+    <col min="9" max="9" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -886,8 +923,14 @@
       <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -907,8 +950,14 @@
         <f>F4*E4</f>
         <v>8.9700000000000006</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -928,8 +977,14 @@
         <f t="shared" ref="G5:G11" si="0">F5*E5</f>
         <v>1.01</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -949,8 +1004,14 @@
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -974,7 +1035,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -998,7 +1059,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1022,7 +1083,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1046,7 +1107,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1070,7 +1131,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1081,7 +1142,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F13" s="3" t="s">
         <v>26</v>
       </c>
@@ -1098,7 +1159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>